<commit_message>
[210625] UPDATE 15_MEMBER UPDATE 쇼핑몰 테이블 정의.xlsx
</commit_message>
<xml_diff>
--- a/쇼핑몰 테이블 정의.xlsx
+++ b/쇼핑몰 테이블 정의.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSH\SpringFrameWork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSH\SpringFrameWork\workplace\ITKOREA_SpringFramework_SPRINGSTUDY\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="144">
   <si>
     <t>객체</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,10 +106,6 @@
   </si>
   <si>
     <t>MEMBER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHOP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -502,6 +498,102 @@
   </si>
   <si>
     <t>VARCHAR2(64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QNA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TABLENAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TABLENAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TABLENAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TABLENAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USERID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QUESTION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POSTDATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MANAGERID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ANSWER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TITLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ANSWERDATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMBER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2(100)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원아이디(FK:MEMBER)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자아이디(FK:MEMBER)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질문제목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질문내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질문작성일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>답변내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>답변작성일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -778,7 +870,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -845,79 +937,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -927,6 +989,51 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1212,10 +1319,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1238,45 +1345,45 @@
       <c r="C1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="39">
+      <c r="G1" s="41"/>
+      <c r="H1" s="42">
         <v>44372</v>
       </c>
-      <c r="I1" s="37"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="41"/>
+      <c r="H2" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="37"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="43"/>
     </row>
     <row r="3" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
@@ -1285,10 +1392,10 @@
       <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1301,23 +1408,23 @@
       <c r="H3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="27"/>
+        <v>22</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="35"/>
       <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1326,172 +1433,172 @@
         <v>15</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="44"/>
+      <c r="I4" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
     </row>
     <row r="5" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="21"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="45"/>
-      <c r="K5" s="46"/>
+      <c r="I5" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="31"/>
+      <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="27"/>
+        <v>24</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="35"/>
       <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
+      <c r="I6" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="21"/>
+        <v>25</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="36"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46"/>
+      <c r="I7" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="31"/>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="21"/>
+        <v>26</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="36"/>
       <c r="E8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46"/>
+      <c r="I8" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>6</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="40"/>
+        <v>27</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="28"/>
       <c r="E9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="41"/>
-      <c r="K9" s="42"/>
+      <c r="I9" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="33"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="40"/>
+        <v>28</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="28"/>
       <c r="E10" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="41"/>
-      <c r="K10" s="42"/>
+      <c r="I10" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="33"/>
+      <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="40"/>
+        <v>29</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="28"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
-      <c r="I11" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" s="41"/>
-      <c r="K11" s="42"/>
+      <c r="I11" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="33"/>
+      <c r="K11" s="34"/>
       <c r="O11" t="s">
         <v>18</v>
       </c>
@@ -1501,84 +1608,84 @@
         <v>9</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="40"/>
+        <v>37</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="28"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
-      <c r="I12" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="41"/>
-      <c r="K12" s="42"/>
+      <c r="I12" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="33"/>
+      <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>10</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="40"/>
+        <v>38</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="28"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="J13" s="48"/>
-      <c r="K13" s="49"/>
+      <c r="I13" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="38"/>
+      <c r="K13" s="39"/>
     </row>
     <row r="14" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
-      <c r="I14" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="41"/>
-      <c r="K14" s="42"/>
+      <c r="I14" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="33"/>
+      <c r="K14" s="34"/>
     </row>
     <row r="15" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15" s="40"/>
+        <v>116</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="28"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
-      <c r="I15" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="42"/>
+      <c r="I15" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="33"/>
+      <c r="K15" s="34"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
@@ -1590,45 +1697,45 @@
       <c r="C18" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33" t="s">
+      <c r="D18" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="39">
+      <c r="G18" s="41"/>
+      <c r="H18" s="42">
         <v>44370</v>
       </c>
-      <c r="I18" s="37"/>
+      <c r="I18" s="43"/>
       <c r="J18" s="13" t="s">
         <v>6</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="37"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="43"/>
     </row>
     <row r="20" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
@@ -1637,10 +1744,10 @@
       <c r="B20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="31"/>
+      <c r="D20" s="26"/>
       <c r="E20" s="13" t="s">
         <v>10</v>
       </c>
@@ -1653,23 +1760,23 @@
       <c r="H20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>1</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="27"/>
+        <v>22</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="35"/>
       <c r="E21" s="15" t="s">
         <v>16</v>
       </c>
@@ -1678,80 +1785,80 @@
         <v>15</v>
       </c>
       <c r="H21" s="14"/>
-      <c r="I21" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" s="43"/>
-      <c r="K21" s="44"/>
+      <c r="I21" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J21" s="29"/>
+      <c r="K21" s="30"/>
     </row>
     <row r="22" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>2</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="21"/>
+      <c r="D22" s="36"/>
       <c r="E22" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I22" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="J22" s="45"/>
-      <c r="K22" s="46"/>
+        <v>36</v>
+      </c>
+      <c r="I22" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="31"/>
+      <c r="K22" s="32"/>
     </row>
     <row r="23" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>3</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="27"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="J23" s="43"/>
-      <c r="K23" s="44"/>
+      <c r="I23" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" s="29"/>
+      <c r="K23" s="30"/>
     </row>
     <row r="24" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="21"/>
+      <c r="D24" s="36"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
-      <c r="I24" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="J24" s="45"/>
-      <c r="K24" s="46"/>
+      <c r="I24" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="31"/>
+      <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
@@ -1776,45 +1883,45 @@
       <c r="C27" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33" t="s">
+      <c r="D27" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="27"/>
+      <c r="F27" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="34"/>
-      <c r="H27" s="39">
+      <c r="G27" s="41"/>
+      <c r="H27" s="42">
         <v>44370</v>
       </c>
-      <c r="I27" s="37"/>
+      <c r="I27" s="43"/>
       <c r="J27" s="13" t="s">
         <v>6</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="33" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="34"/>
-      <c r="H28" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="37"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="43"/>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
@@ -1823,10 +1930,10 @@
       <c r="B29" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="31"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="13" t="s">
         <v>10</v>
       </c>
@@ -1839,23 +1946,23 @@
       <c r="H29" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="33" t="s">
+      <c r="I29" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="J29" s="38"/>
-      <c r="K29" s="34"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="41"/>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>1</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="27"/>
+        <v>22</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="35"/>
       <c r="E30" s="15" t="s">
         <v>16</v>
       </c>
@@ -1864,122 +1971,122 @@
         <v>15</v>
       </c>
       <c r="H30" s="14"/>
-      <c r="I30" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="J30" s="29"/>
-      <c r="K30" s="30"/>
+      <c r="I30" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" s="48"/>
+      <c r="K30" s="49"/>
     </row>
     <row r="31" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>2</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="21"/>
+      <c r="D31" s="36"/>
       <c r="E31" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I31" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="J31" s="23"/>
-      <c r="K31" s="24"/>
+        <v>36</v>
+      </c>
+      <c r="I31" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="J31" s="51"/>
+      <c r="K31" s="52"/>
     </row>
     <row r="32" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>3</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="26"/>
+        <v>71</v>
+      </c>
+      <c r="C32" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="54"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
-      <c r="I32" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J32" s="29"/>
-      <c r="K32" s="30"/>
+      <c r="I32" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="J32" s="48"/>
+      <c r="K32" s="49"/>
     </row>
     <row r="33" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17">
         <v>4</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="26"/>
+        <v>30</v>
+      </c>
+      <c r="C33" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="54"/>
       <c r="E33" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
-      <c r="I33" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="J33" s="23"/>
-      <c r="K33" s="24"/>
+      <c r="I33" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" s="51"/>
+      <c r="K33" s="52"/>
     </row>
     <row r="34" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17">
         <v>5</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="26"/>
+        <v>31</v>
+      </c>
+      <c r="C34" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="54"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
-      <c r="I34" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="J34" s="23"/>
-      <c r="K34" s="24"/>
+      <c r="I34" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="J34" s="51"/>
+      <c r="K34" s="52"/>
     </row>
     <row r="35" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17">
         <v>6</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="21"/>
+      <c r="D35" s="36"/>
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
-      <c r="I35" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="J35" s="23"/>
-      <c r="K35" s="24"/>
+      <c r="I35" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="J35" s="51"/>
+      <c r="K35" s="52"/>
     </row>
     <row r="36" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
@@ -2004,45 +2111,45 @@
       <c r="C38" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="32"/>
-      <c r="F38" s="33" t="s">
+      <c r="D38" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="27"/>
+      <c r="F38" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="34"/>
-      <c r="H38" s="39">
+      <c r="G38" s="41"/>
+      <c r="H38" s="42">
         <v>44370</v>
       </c>
-      <c r="I38" s="37"/>
+      <c r="I38" s="43"/>
       <c r="J38" s="13" t="s">
         <v>6</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33" t="s">
+      <c r="B39" s="26"/>
+      <c r="C39" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G39" s="34"/>
-      <c r="H39" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="37"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="43"/>
     </row>
     <row r="40" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
@@ -2051,10 +2158,10 @@
       <c r="B40" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="31"/>
+      <c r="D40" s="26"/>
       <c r="E40" s="13" t="s">
         <v>10</v>
       </c>
@@ -2067,23 +2174,23 @@
       <c r="H40" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="33" t="s">
+      <c r="I40" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="J40" s="38"/>
-      <c r="K40" s="34"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="41"/>
     </row>
     <row r="41" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17">
         <v>1</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" s="27"/>
+        <v>22</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="35"/>
       <c r="E41" s="15" t="s">
         <v>16</v>
       </c>
@@ -2092,162 +2199,162 @@
         <v>15</v>
       </c>
       <c r="H41" s="14"/>
-      <c r="I41" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="J41" s="29"/>
-      <c r="K41" s="30"/>
+      <c r="I41" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="J41" s="48"/>
+      <c r="K41" s="49"/>
     </row>
     <row r="42" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>3</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="26"/>
+      <c r="D42" s="54"/>
       <c r="E42" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
-      <c r="I42" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="J42" s="23"/>
-      <c r="K42" s="24"/>
+      <c r="I42" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="J42" s="51"/>
+      <c r="K42" s="52"/>
     </row>
     <row r="43" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17">
         <v>4</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="26"/>
+        <v>85</v>
+      </c>
+      <c r="C43" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="54"/>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
-      <c r="I43" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="J43" s="23"/>
-      <c r="K43" s="24"/>
+      <c r="I43" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="J43" s="51"/>
+      <c r="K43" s="52"/>
     </row>
     <row r="44" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17">
         <v>5</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="26"/>
+        <v>95</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="54"/>
       <c r="E44" s="15"/>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
-      <c r="I44" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="J44" s="23"/>
-      <c r="K44" s="24"/>
+      <c r="I44" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="J44" s="51"/>
+      <c r="K44" s="52"/>
     </row>
     <row r="45" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17">
         <v>6</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" s="26"/>
+        <v>94</v>
+      </c>
+      <c r="C45" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="54"/>
       <c r="E45" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
-      <c r="I45" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="J45" s="23"/>
-      <c r="K45" s="24"/>
+      <c r="I45" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="J45" s="51"/>
+      <c r="K45" s="52"/>
     </row>
     <row r="46" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="17">
         <v>7</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="21"/>
+      <c r="D46" s="36"/>
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
-      <c r="I46" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="J46" s="23"/>
-      <c r="K46" s="24"/>
+      <c r="I46" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="J46" s="51"/>
+      <c r="K46" s="52"/>
     </row>
     <row r="47" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="17">
         <v>8</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47" s="21"/>
+        <v>69</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="36"/>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
-      <c r="I47" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="J47" s="23"/>
-      <c r="K47" s="24"/>
+      <c r="I47" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="J47" s="51"/>
+      <c r="K47" s="52"/>
     </row>
     <row r="48" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17">
         <v>9</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D48" s="21"/>
+      <c r="D48" s="36"/>
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
-      <c r="I48" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="J48" s="23"/>
-      <c r="K48" s="24"/>
+      <c r="I48" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="J48" s="51"/>
+      <c r="K48" s="52"/>
     </row>
     <row r="49" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19"/>
@@ -2272,45 +2379,45 @@
       <c r="C51" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="E51" s="32"/>
-      <c r="F51" s="33" t="s">
+      <c r="D51" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" s="27"/>
+      <c r="F51" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G51" s="34"/>
-      <c r="H51" s="39">
+      <c r="G51" s="41"/>
+      <c r="H51" s="42">
         <v>44370</v>
       </c>
-      <c r="I51" s="37"/>
+      <c r="I51" s="43"/>
       <c r="J51" s="13" t="s">
         <v>6</v>
       </c>
       <c r="K51" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="33" t="s">
+      <c r="B52" s="26"/>
+      <c r="C52" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G52" s="34"/>
-      <c r="H52" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="I52" s="36"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="37"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="I52" s="45"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="43"/>
     </row>
     <row r="53" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
@@ -2319,10 +2426,10 @@
       <c r="B53" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="31" t="s">
+      <c r="C53" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="31"/>
+      <c r="D53" s="26"/>
       <c r="E53" s="13" t="s">
         <v>10</v>
       </c>
@@ -2335,23 +2442,23 @@
       <c r="H53" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I53" s="33" t="s">
+      <c r="I53" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="J53" s="38"/>
-      <c r="K53" s="34"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="41"/>
     </row>
     <row r="54" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="17">
         <v>1</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D54" s="27"/>
+        <v>22</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="35"/>
       <c r="E54" s="15" t="s">
         <v>16</v>
       </c>
@@ -2360,234 +2467,454 @@
         <v>15</v>
       </c>
       <c r="H54" s="14"/>
-      <c r="I54" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="J54" s="29"/>
-      <c r="K54" s="30"/>
+      <c r="I54" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="J54" s="48"/>
+      <c r="K54" s="49"/>
     </row>
     <row r="55" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>2</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C55" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D55" s="26"/>
+        <v>104</v>
+      </c>
+      <c r="C55" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="D55" s="54"/>
       <c r="E55" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
       <c r="H55" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I55" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="J55" s="23"/>
-      <c r="K55" s="24"/>
+        <v>36</v>
+      </c>
+      <c r="I55" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="J55" s="51"/>
+      <c r="K55" s="52"/>
     </row>
     <row r="56" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17">
         <v>3</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="D56" s="26"/>
+        <v>82</v>
+      </c>
+      <c r="C56" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="54"/>
       <c r="E56" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
       <c r="H56" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I56" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="J56" s="23"/>
-      <c r="K56" s="24"/>
+        <v>36</v>
+      </c>
+      <c r="I56" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="J56" s="51"/>
+      <c r="K56" s="52"/>
     </row>
     <row r="57" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17">
         <v>4</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C57" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D57" s="26"/>
+        <v>84</v>
+      </c>
+      <c r="C57" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" s="54"/>
       <c r="E57" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
-      <c r="I57" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="J57" s="23"/>
-      <c r="K57" s="24"/>
+      <c r="I57" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="J57" s="51"/>
+      <c r="K57" s="52"/>
     </row>
     <row r="58" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="17">
         <v>5</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D58" s="26"/>
+        <v>94</v>
+      </c>
+      <c r="C58" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D58" s="54"/>
       <c r="E58" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
       <c r="H58" s="15"/>
-      <c r="I58" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="J58" s="23"/>
-      <c r="K58" s="24"/>
+      <c r="I58" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="J58" s="51"/>
+      <c r="K58" s="52"/>
     </row>
     <row r="59" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="17">
         <v>6</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C59" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="21"/>
+      <c r="D59" s="36"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
-      <c r="I59" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="J59" s="23"/>
-      <c r="K59" s="24"/>
+      <c r="I59" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="J59" s="51"/>
+      <c r="K59" s="52"/>
     </row>
     <row r="60" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="17">
         <v>7</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D60" s="21"/>
+        <v>69</v>
+      </c>
+      <c r="C60" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="36"/>
       <c r="E60" s="15"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
-      <c r="I60" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="J60" s="23"/>
-      <c r="K60" s="24"/>
+      <c r="I60" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="J60" s="51"/>
+      <c r="K60" s="52"/>
+    </row>
+    <row r="63" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E63" s="27"/>
+      <c r="F63" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="G63" s="41"/>
+      <c r="H63" s="42">
+        <v>44372</v>
+      </c>
+      <c r="I63" s="43"/>
+      <c r="J63" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K63" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="26"/>
+      <c r="C64" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="41"/>
+      <c r="H64" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="I64" s="45"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="43"/>
+    </row>
+    <row r="65" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" s="26"/>
+      <c r="E65" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G65" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I65" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65" s="46"/>
+      <c r="K65" s="41"/>
+    </row>
+    <row r="66" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="25">
+        <v>1</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" s="35"/>
+      <c r="E66" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="H66" s="23"/>
+      <c r="I66" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="J66" s="48"/>
+      <c r="K66" s="49"/>
+    </row>
+    <row r="67" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="5">
+        <v>2</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="36"/>
+      <c r="E67" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I67" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="J67" s="51"/>
+      <c r="K67" s="52"/>
+    </row>
+    <row r="68" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="25">
+        <v>3</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="53" t="s">
+        <v>134</v>
+      </c>
+      <c r="D68" s="54"/>
+      <c r="E68" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="J68" s="51"/>
+      <c r="K68" s="52"/>
+    </row>
+    <row r="69" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="25">
+        <v>3</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C69" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="54"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="J69" s="51"/>
+      <c r="K69" s="52"/>
+    </row>
+    <row r="70" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="25">
+        <v>4</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="54"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="J70" s="51"/>
+      <c r="K70" s="52"/>
+    </row>
+    <row r="71" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="25">
+        <v>5</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="36"/>
+      <c r="E71" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I71" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="J71" s="51"/>
+      <c r="K71" s="52"/>
+    </row>
+    <row r="72" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="25">
+        <v>6</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C72" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" s="54"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="J72" s="51"/>
+      <c r="K72" s="52"/>
+    </row>
+    <row r="73" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="25">
+        <v>8</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D73" s="54"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="J73" s="51"/>
+      <c r="K73" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="119">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:K39"/>
+  <mergeCells count="144">
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="I71:K71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="I73:K73"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="I66:K66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="I67:K67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="I68:K68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="I69:K69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="I70:K70"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="H64:K64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="I65:K65"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="I60:K60"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="I56:K56"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="F52:G52"/>
@@ -2609,22 +2936,88 @@
     <mergeCell ref="I43:K43"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="I45:K45"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="I60:K60"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="I59:K59"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[210701]UPDATE 17_SEARCH ADD IntegrationProject
</commit_message>
<xml_diff>
--- a/쇼핑몰 테이블 정의.xlsx
+++ b/쇼핑몰 테이블 정의.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="202">
   <si>
     <t>객체</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,10 +118,6 @@
   </si>
   <si>
     <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -818,6 +814,18 @@
   </si>
   <si>
     <t>상태(취소:-2 ,환불:-1, 주문됨:0, 배송중:1, 배송완료:2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDRESS_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>받는사람이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1082,7 +1090,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1167,6 +1175,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1176,12 +1205,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,6 +1217,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1224,22 +1250,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1249,15 +1275,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1549,10 +1566,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O98"/>
+  <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:K15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1575,18 +1592,18 @@
       <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="38" t="s">
+      <c r="E1" s="43"/>
+      <c r="F1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40">
+      <c r="G1" s="45"/>
+      <c r="H1" s="46">
         <v>44372</v>
       </c>
-      <c r="I1" s="41"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
@@ -1595,25 +1612,25 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="43" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="41"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
@@ -1622,10 +1639,10 @@
       <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1638,23 +1655,23 @@
       <c r="H3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="33"/>
+        <v>137</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="38"/>
       <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1663,172 +1680,170 @@
         <v>15</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="50"/>
+      <c r="I4" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="53"/>
+      <c r="K4" s="54"/>
     </row>
     <row r="5" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="51"/>
-      <c r="K5" s="52"/>
+      <c r="I5" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="55"/>
+      <c r="K5" s="56"/>
     </row>
     <row r="6" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="33"/>
+        <v>139</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="38"/>
       <c r="E6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="J6" s="49"/>
-      <c r="K6" s="50"/>
+      <c r="I6" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="53"/>
+      <c r="K6" s="54"/>
     </row>
     <row r="7" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="27"/>
+        <v>140</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="42"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
+      <c r="I7" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="55"/>
+      <c r="K7" s="56"/>
     </row>
     <row r="8" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="4" t="s">
-        <v>26</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
+      <c r="I8" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="55"/>
+      <c r="K8" s="56"/>
     </row>
     <row r="9" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="46"/>
+        <v>142</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="52"/>
       <c r="E9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="48"/>
+      <c r="I9" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
     </row>
     <row r="10" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="46"/>
+        <v>143</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="52"/>
       <c r="E10" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="48"/>
+      <c r="I10" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="57"/>
+      <c r="K10" s="58"/>
     </row>
     <row r="11" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="46"/>
+        <v>144</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="52"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48"/>
+      <c r="I11" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58"/>
       <c r="O11" t="s">
         <v>18</v>
       </c>
@@ -1838,86 +1853,86 @@
         <v>9</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="46"/>
+        <v>145</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="52"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="47"/>
-      <c r="K12" s="48"/>
+      <c r="I12" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="57"/>
+      <c r="K12" s="58"/>
     </row>
     <row r="13" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>10</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="46"/>
+        <v>146</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="52"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="55"/>
+      <c r="I13" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="60"/>
+      <c r="K13" s="61"/>
     </row>
     <row r="14" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>11</v>
       </c>
       <c r="B14" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="46"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="J14" s="47"/>
-      <c r="K14" s="48"/>
+      <c r="I14" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="57"/>
+      <c r="K14" s="58"/>
     </row>
     <row r="15" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="56">
+      <c r="A15" s="30">
         <v>12</v>
       </c>
-      <c r="B15" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" s="58" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="58" t="s">
+      <c r="B15" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="58"/>
-      <c r="K15" s="60"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" s="62"/>
+      <c r="K15" s="63"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
@@ -1929,18 +1944,18 @@
       <c r="C18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38" t="s">
+      <c r="D18" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="43"/>
+      <c r="F18" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40">
+      <c r="G18" s="45"/>
+      <c r="H18" s="46">
         <v>44370</v>
       </c>
-      <c r="I18" s="41"/>
+      <c r="I18" s="47"/>
       <c r="J18" s="10" t="s">
         <v>6</v>
       </c>
@@ -1949,25 +1964,25 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38" t="s">
+      <c r="B19" s="48"/>
+      <c r="C19" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="41"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="47"/>
     </row>
     <row r="20" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -1976,10 +1991,10 @@
       <c r="B20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="42"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="10" t="s">
         <v>10</v>
       </c>
@@ -1992,23 +2007,23 @@
       <c r="H20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="42" t="s">
+      <c r="I20" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
     </row>
     <row r="21" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>1</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="33"/>
+        <v>125</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="38"/>
       <c r="E21" s="12" t="s">
         <v>16</v>
       </c>
@@ -2017,82 +2032,82 @@
         <v>15</v>
       </c>
       <c r="H21" s="11"/>
-      <c r="I21" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="J21" s="49"/>
-      <c r="K21" s="50"/>
+      <c r="I21" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="53"/>
+      <c r="K21" s="54"/>
     </row>
     <row r="22" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <v>2</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C22" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="27"/>
+      <c r="D22" s="42"/>
       <c r="E22" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" s="51"/>
-      <c r="K22" s="52"/>
+        <v>27</v>
+      </c>
+      <c r="I22" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" s="55"/>
+      <c r="K22" s="56"/>
     </row>
     <row r="23" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>3</v>
       </c>
       <c r="B23" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="33"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="49"/>
-      <c r="K23" s="50"/>
+      <c r="I23" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="J23" s="53"/>
+      <c r="K23" s="54"/>
     </row>
     <row r="24" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <v>4</v>
       </c>
       <c r="B24" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="42"/>
       <c r="E24" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="J24" s="51"/>
-      <c r="K24" s="52"/>
+      <c r="I24" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="55"/>
+      <c r="K24" s="56"/>
     </row>
     <row r="25" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
@@ -2117,18 +2132,18 @@
       <c r="C27" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38" t="s">
+      <c r="D27" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="43"/>
+      <c r="F27" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40">
+      <c r="G27" s="45"/>
+      <c r="H27" s="46">
         <v>44370</v>
       </c>
-      <c r="I27" s="41"/>
+      <c r="I27" s="47"/>
       <c r="J27" s="10" t="s">
         <v>6</v>
       </c>
@@ -2137,25 +2152,25 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38" t="s">
+      <c r="B28" s="48"/>
+      <c r="C28" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="39"/>
-      <c r="H28" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="41"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="47"/>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
@@ -2164,10 +2179,10 @@
       <c r="B29" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="42"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="10" t="s">
         <v>10</v>
       </c>
@@ -2180,23 +2195,23 @@
       <c r="H29" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="38" t="s">
+      <c r="I29" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="J29" s="45"/>
-      <c r="K29" s="39"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="45"/>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>1</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="33"/>
+        <v>131</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="38"/>
       <c r="E30" s="12" t="s">
         <v>16</v>
       </c>
@@ -2205,1478 +2220,1584 @@
         <v>15</v>
       </c>
       <c r="H30" s="11"/>
-      <c r="I30" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="J30" s="35"/>
-      <c r="K30" s="36"/>
+      <c r="I30" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J30" s="40"/>
+      <c r="K30" s="41"/>
     </row>
     <row r="31" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
         <v>2</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="C31" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="27"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="J31" s="29"/>
-      <c r="K31" s="30"/>
+        <v>27</v>
+      </c>
+      <c r="I31" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="J31" s="36"/>
+      <c r="K31" s="37"/>
     </row>
     <row r="32" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>3</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="32"/>
+        <v>199</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="34"/>
       <c r="E32" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
-      <c r="I32" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="J32" s="35"/>
-      <c r="K32" s="36"/>
+      <c r="I32" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="J32" s="40"/>
+      <c r="K32" s="41"/>
     </row>
     <row r="33" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14">
+      <c r="A33" s="29">
         <v>4</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="32"/>
-      <c r="E33" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="J33" s="29"/>
-      <c r="K33" s="30"/>
+      <c r="B33" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="42"/>
+      <c r="E33" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="J33" s="36"/>
+      <c r="K33" s="37"/>
     </row>
     <row r="34" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
         <v>5</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="32"/>
-      <c r="E34" s="12"/>
+        <v>133</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="34"/>
+      <c r="E34" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
-      <c r="I34" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="J34" s="29"/>
-      <c r="K34" s="30"/>
+      <c r="I34" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="J34" s="36"/>
+      <c r="K34" s="37"/>
     </row>
     <row r="35" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
         <v>6</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="27"/>
+        <v>134</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="34"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="28" t="s">
+      <c r="I35" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J35" s="36"/>
+      <c r="K35" s="37"/>
+    </row>
+    <row r="36" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>7</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="42"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="J36" s="36"/>
+      <c r="K36" s="37"/>
+    </row>
+    <row r="37" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+    </row>
+    <row r="39" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="J35" s="29"/>
-      <c r="K35" s="30"/>
-    </row>
-    <row r="36" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-    </row>
-    <row r="38" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="14" t="s">
+      <c r="E39" s="43"/>
+      <c r="F39" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="45"/>
+      <c r="H39" s="46">
+        <v>44370</v>
+      </c>
+      <c r="I39" s="47"/>
+      <c r="J39" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="48"/>
+      <c r="C40" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="45"/>
+      <c r="H40" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="I40" s="50"/>
+      <c r="J40" s="50"/>
+      <c r="K40" s="47"/>
+    </row>
+    <row r="41" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="48"/>
+      <c r="E41" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="51"/>
+      <c r="K41" s="45"/>
+    </row>
+    <row r="42" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14">
+        <v>1</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="38"/>
+      <c r="E42" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="11"/>
+      <c r="I42" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="J42" s="40"/>
+      <c r="K42" s="41"/>
+    </row>
+    <row r="43" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
         <v>3</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" s="37"/>
-      <c r="F38" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G38" s="39"/>
-      <c r="H38" s="40">
-        <v>44370</v>
-      </c>
-      <c r="I38" s="41"/>
-      <c r="J38" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K38" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="42"/>
-      <c r="C39" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="39"/>
-      <c r="H39" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="41"/>
-    </row>
-    <row r="40" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="42"/>
-      <c r="E40" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I40" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="J40" s="45"/>
-      <c r="K40" s="39"/>
-    </row>
-    <row r="41" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="14">
-        <v>1</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="33"/>
-      <c r="E41" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="J41" s="35"/>
-      <c r="K41" s="36"/>
-    </row>
-    <row r="42" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
-        <v>3</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="32"/>
-      <c r="E42" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="J42" s="29"/>
-      <c r="K42" s="30"/>
-    </row>
-    <row r="43" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="14">
-        <v>4</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D43" s="32"/>
-      <c r="E43" s="12"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
-      <c r="I43" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J43" s="29"/>
-      <c r="K43" s="30"/>
+      <c r="I43" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="J43" s="36"/>
+      <c r="K43" s="37"/>
     </row>
     <row r="44" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="32"/>
+      <c r="C44" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="34"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="J44" s="29"/>
-      <c r="K44" s="30"/>
+      <c r="I44" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="J44" s="36"/>
+      <c r="K44" s="37"/>
     </row>
     <row r="45" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="32"/>
-      <c r="E45" s="12" t="s">
-        <v>26</v>
-      </c>
+      <c r="C45" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="34"/>
+      <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
-      <c r="I45" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="J45" s="29"/>
-      <c r="K45" s="30"/>
+      <c r="I45" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="J45" s="36"/>
+      <c r="K45" s="37"/>
     </row>
     <row r="46" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" s="27"/>
-      <c r="E46" s="12"/>
+        <v>81</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" s="34"/>
+      <c r="E46" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="J46" s="29"/>
-      <c r="K46" s="30"/>
+      <c r="I46" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="J46" s="36"/>
+      <c r="K46" s="37"/>
     </row>
     <row r="47" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" s="27"/>
+        <v>77</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="42"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
-      <c r="I47" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="J47" s="29"/>
-      <c r="K47" s="30"/>
+      <c r="I47" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="J47" s="36"/>
+      <c r="K47" s="37"/>
     </row>
     <row r="48" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" s="27"/>
+        <v>59</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" s="42"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
-      <c r="I48" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="J48" s="29"/>
-      <c r="K48" s="30"/>
+      <c r="I48" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="J48" s="36"/>
+      <c r="K48" s="37"/>
     </row>
     <row r="49" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-    </row>
-    <row r="51" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="s">
+      <c r="A49" s="14">
+        <v>9</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" s="42"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="J49" s="36"/>
+      <c r="K49" s="37"/>
+    </row>
+    <row r="50" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+    </row>
+    <row r="52" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B52" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C52" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="37" t="s">
+      <c r="D52" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52" s="43"/>
+      <c r="F52" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" s="45"/>
+      <c r="H52" s="46">
+        <v>44370</v>
+      </c>
+      <c r="I52" s="47"/>
+      <c r="J52" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K52" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="48"/>
+      <c r="C53" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="45"/>
+      <c r="H53" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="E51" s="37"/>
-      <c r="F51" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="39"/>
-      <c r="H51" s="40">
-        <v>44370</v>
-      </c>
-      <c r="I51" s="41"/>
-      <c r="J51" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K51" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="42" t="s">
+      <c r="I53" s="50"/>
+      <c r="J53" s="50"/>
+      <c r="K53" s="47"/>
+    </row>
+    <row r="54" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="48"/>
+      <c r="E54" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" s="51"/>
+      <c r="K54" s="45"/>
+    </row>
+    <row r="55" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="14">
         <v>1</v>
       </c>
-      <c r="B52" s="42"/>
-      <c r="C52" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52" s="39"/>
-      <c r="H52" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="I52" s="44"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="41"/>
-    </row>
-    <row r="53" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="s">
+      <c r="B55" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="38"/>
+      <c r="E55" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="11"/>
+      <c r="I55" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="J55" s="40"/>
+      <c r="K55" s="41"/>
+    </row>
+    <row r="56" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
         <v>2</v>
       </c>
-      <c r="B53" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="42"/>
-      <c r="E53" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I53" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="J53" s="45"/>
-      <c r="K53" s="39"/>
-    </row>
-    <row r="54" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="14">
-        <v>1</v>
-      </c>
-      <c r="B54" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C54" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="33"/>
-      <c r="E54" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H54" s="11"/>
-      <c r="I54" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="J54" s="35"/>
-      <c r="K54" s="36"/>
-    </row>
-    <row r="55" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="5">
-        <v>2</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C55" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D55" s="32"/>
-      <c r="E55" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I55" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="J55" s="29"/>
-      <c r="K55" s="30"/>
-    </row>
-    <row r="56" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="14">
-        <v>3</v>
-      </c>
       <c r="B56" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C56" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D56" s="32"/>
+        <v>130</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" s="34"/>
       <c r="E56" s="12" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I56" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="J56" s="29"/>
-      <c r="K56" s="30"/>
+        <v>27</v>
+      </c>
+      <c r="I56" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="J56" s="36"/>
+      <c r="K56" s="37"/>
     </row>
     <row r="57" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D57" s="32"/>
+        <v>22</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" s="34"/>
       <c r="E57" s="12" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="J57" s="29"/>
-      <c r="K57" s="30"/>
+      <c r="H57" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="J57" s="36"/>
+      <c r="K57" s="37"/>
     </row>
     <row r="58" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C58" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D58" s="32"/>
+      <c r="C58" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" s="34"/>
       <c r="E58" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
-      <c r="I58" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="J58" s="29"/>
-      <c r="K58" s="30"/>
+      <c r="I58" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="J58" s="36"/>
+      <c r="K58" s="37"/>
     </row>
     <row r="59" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="C59" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D59" s="27"/>
-      <c r="E59" s="12"/>
+        <v>81</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" s="34"/>
+      <c r="E59" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="J59" s="29"/>
-      <c r="K59" s="30"/>
+      <c r="I59" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="J59" s="36"/>
+      <c r="K59" s="37"/>
     </row>
     <row r="60" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="23">
-        <v>7</v>
+      <c r="A60" s="14">
+        <v>6</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D60" s="27"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="J60" s="29"/>
-      <c r="K60" s="30"/>
+        <v>149</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="42"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="J60" s="36"/>
+      <c r="K60" s="37"/>
     </row>
     <row r="61" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="C61" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" s="27"/>
-      <c r="E61" s="25" t="s">
-        <v>159</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C61" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" s="42"/>
+      <c r="E61" s="25"/>
       <c r="F61" s="25"/>
       <c r="G61" s="25"/>
-      <c r="H61" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="I61" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="J61" s="29"/>
-      <c r="K61" s="30"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="J61" s="36"/>
+      <c r="K61" s="37"/>
     </row>
     <row r="62" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="23">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="C62" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="D62" s="27"/>
+        <v>171</v>
+      </c>
+      <c r="C62" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D62" s="42"/>
       <c r="E62" s="25" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="F62" s="25"/>
       <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="J62" s="29"/>
-      <c r="K62" s="30"/>
+      <c r="H62" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="I62" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="J62" s="36"/>
+      <c r="K62" s="37"/>
     </row>
     <row r="63" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="14">
+      <c r="A63" s="23">
+        <v>9</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C63" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D63" s="42"/>
+      <c r="E63" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="25"/>
+      <c r="G63" s="25"/>
+      <c r="H63" s="25"/>
+      <c r="I63" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="J63" s="36"/>
+      <c r="K63" s="37"/>
+    </row>
+    <row r="64" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="14">
         <v>10</v>
       </c>
-      <c r="B63" s="26" t="s">
+      <c r="B64" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="C63" s="27" t="s">
+      <c r="D64" s="42"/>
+      <c r="E64" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="D63" s="27"/>
-      <c r="E63" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="J63" s="29"/>
-      <c r="K63" s="30"/>
-    </row>
-    <row r="66" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="20" t="s">
+      <c r="J64" s="36"/>
+      <c r="K64" s="37"/>
+    </row>
+    <row r="67" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="21" t="s">
+      <c r="B67" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C67" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="E66" s="37"/>
-      <c r="F66" s="38" t="s">
+      <c r="D67" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E67" s="43"/>
+      <c r="F67" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G66" s="39"/>
-      <c r="H66" s="40">
+      <c r="G67" s="45"/>
+      <c r="H67" s="46">
         <v>44372</v>
       </c>
-      <c r="I66" s="41"/>
-      <c r="J66" s="20" t="s">
+      <c r="I67" s="47"/>
+      <c r="J67" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K66" s="21" t="s">
+      <c r="K67" s="21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="42" t="s">
+    <row r="68" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="42"/>
-      <c r="C67" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="38" t="s">
+      <c r="B68" s="48"/>
+      <c r="C68" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D68" s="43"/>
+      <c r="E68" s="43"/>
+      <c r="F68" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G67" s="39"/>
-      <c r="H67" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="I67" s="44"/>
-      <c r="J67" s="44"/>
-      <c r="K67" s="41"/>
-    </row>
-    <row r="68" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="20" t="s">
+      <c r="G68" s="45"/>
+      <c r="H68" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="I68" s="50"/>
+      <c r="J68" s="50"/>
+      <c r="K68" s="47"/>
+    </row>
+    <row r="69" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B69" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C68" s="42" t="s">
+      <c r="C69" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="42"/>
-      <c r="E68" s="20" t="s">
+      <c r="D69" s="48"/>
+      <c r="E69" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F68" s="20" t="s">
+      <c r="F69" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G68" s="20" t="s">
+      <c r="G69" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H68" s="20" t="s">
+      <c r="H69" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I68" s="38" t="s">
+      <c r="I69" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="J68" s="45"/>
-      <c r="K68" s="39"/>
-    </row>
-    <row r="69" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="21">
+      <c r="J69" s="51"/>
+      <c r="K69" s="45"/>
+    </row>
+    <row r="70" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="21">
         <v>1</v>
       </c>
-      <c r="B69" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="C69" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="D69" s="33"/>
-      <c r="E69" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="H69" s="19"/>
-      <c r="I69" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="J69" s="35"/>
-      <c r="K69" s="36"/>
-    </row>
-    <row r="70" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="5">
-        <v>2</v>
-      </c>
-      <c r="B70" s="18" t="s">
+      <c r="B70" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="C70" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70" s="27"/>
+      <c r="C70" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" s="38"/>
       <c r="E70" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="I70" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="J70" s="29"/>
-      <c r="K70" s="30"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="H70" s="19"/>
+      <c r="I70" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J70" s="40"/>
+      <c r="K70" s="41"/>
     </row>
     <row r="71" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="21">
-        <v>3</v>
+      <c r="A71" s="5">
+        <v>2</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="C71" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="D71" s="32"/>
+        <v>128</v>
+      </c>
+      <c r="C71" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="42"/>
       <c r="E71" s="17" t="s">
         <v>16</v>
       </c>
       <c r="F71" s="17"/>
       <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="J71" s="29"/>
-      <c r="K71" s="30"/>
+      <c r="H71" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I71" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="J71" s="36"/>
+      <c r="K71" s="37"/>
     </row>
     <row r="72" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="21">
         <v>3</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C72" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D72" s="32"/>
+        <v>113</v>
+      </c>
+      <c r="C72" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="D72" s="34"/>
       <c r="E72" s="17" t="s">
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="17"/>
       <c r="H72" s="17"/>
-      <c r="I72" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="J72" s="29"/>
-      <c r="K72" s="30"/>
+      <c r="I72" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="J72" s="36"/>
+      <c r="K72" s="37"/>
     </row>
     <row r="73" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C73" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D73" s="32"/>
-      <c r="E73" s="17"/>
+        <v>110</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D73" s="34"/>
+      <c r="E73" s="17" t="s">
+        <v>158</v>
+      </c>
       <c r="F73" s="17"/>
       <c r="G73" s="17"/>
       <c r="H73" s="17"/>
-      <c r="I73" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J73" s="29"/>
-      <c r="K73" s="30"/>
+      <c r="I73" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="J73" s="36"/>
+      <c r="K73" s="37"/>
     </row>
     <row r="74" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="C74" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D74" s="27"/>
-      <c r="E74" s="17" t="s">
-        <v>16</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C74" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="D74" s="34"/>
+      <c r="E74" s="17"/>
       <c r="F74" s="17"/>
       <c r="G74" s="17"/>
-      <c r="H74" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="I74" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="J74" s="29"/>
-      <c r="K74" s="30"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="J74" s="36"/>
+      <c r="K74" s="37"/>
     </row>
     <row r="75" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C75" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D75" s="32"/>
+        <v>150</v>
+      </c>
+      <c r="C75" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="42"/>
       <c r="E75" s="17" t="s">
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="J75" s="29"/>
-      <c r="K75" s="30"/>
+      <c r="H75" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I75" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="J75" s="36"/>
+      <c r="K75" s="37"/>
     </row>
     <row r="76" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="C76" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D76" s="32"/>
-      <c r="E76" s="17"/>
+        <v>112</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D76" s="34"/>
+      <c r="E76" s="17" t="s">
+        <v>158</v>
+      </c>
       <c r="F76" s="17"/>
       <c r="G76" s="17"/>
       <c r="H76" s="17"/>
-      <c r="I76" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="J76" s="29"/>
-      <c r="K76" s="30"/>
-    </row>
-    <row r="79" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="22" t="s">
+      <c r="I76" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="J76" s="36"/>
+      <c r="K76" s="37"/>
+    </row>
+    <row r="77" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="21">
+        <v>8</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C77" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="D77" s="34"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="J77" s="36"/>
+      <c r="K77" s="37"/>
+    </row>
+    <row r="80" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B80" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C79" s="22" t="s">
+      <c r="C80" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D79" s="37" t="s">
+      <c r="D80" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="E80" s="43"/>
+      <c r="F80" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G80" s="45"/>
+      <c r="H80" s="46">
+        <v>44377</v>
+      </c>
+      <c r="I80" s="47"/>
+      <c r="J80" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="K80" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="48"/>
+      <c r="C81" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D81" s="43"/>
+      <c r="E81" s="43"/>
+      <c r="F81" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G81" s="45"/>
+      <c r="H81" s="49" t="s">
+        <v>167</v>
+      </c>
+      <c r="I81" s="50"/>
+      <c r="J81" s="50"/>
+      <c r="K81" s="47"/>
+    </row>
+    <row r="82" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="48"/>
+      <c r="E82" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G82" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H82" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I82" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="J82" s="51"/>
+      <c r="K82" s="45"/>
+    </row>
+    <row r="83" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="23">
+        <v>1</v>
+      </c>
+      <c r="B83" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="E79" s="37"/>
-      <c r="F79" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G79" s="39"/>
-      <c r="H79" s="40">
-        <v>44377</v>
-      </c>
-      <c r="I79" s="41"/>
-      <c r="J79" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="K79" s="23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B80" s="42"/>
-      <c r="C80" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G80" s="39"/>
-      <c r="H80" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="I80" s="44"/>
-      <c r="J80" s="44"/>
-      <c r="K80" s="41"/>
-    </row>
-    <row r="81" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B81" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D81" s="42"/>
-      <c r="E81" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G81" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H81" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="J81" s="45"/>
-      <c r="K81" s="39"/>
-    </row>
-    <row r="82" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="23">
-        <v>1</v>
-      </c>
-      <c r="B82" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C82" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D82" s="33"/>
-      <c r="E82" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F82" s="24"/>
-      <c r="G82" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="H82" s="24"/>
-      <c r="I82" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="J82" s="35"/>
-      <c r="K82" s="36"/>
-    </row>
-    <row r="83" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="5">
-        <v>2</v>
-      </c>
-      <c r="B83" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="C83" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D83" s="27"/>
+      <c r="C83" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D83" s="38"/>
       <c r="E83" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F83" s="25"/>
-      <c r="G83" s="25"/>
-      <c r="H83" s="25"/>
-      <c r="I83" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="J83" s="29"/>
-      <c r="K83" s="30"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H83" s="24"/>
+      <c r="I83" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J83" s="40"/>
+      <c r="K83" s="41"/>
     </row>
     <row r="84" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="23">
-        <v>3</v>
+      <c r="A84" s="5">
+        <v>2</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="C84" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D84" s="32"/>
+        <v>151</v>
+      </c>
+      <c r="C84" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="42"/>
       <c r="E84" s="25" t="s">
         <v>16</v>
       </c>
       <c r="F84" s="25"/>
       <c r="G84" s="25"/>
       <c r="H84" s="25"/>
-      <c r="I84" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="J84" s="29"/>
-      <c r="K84" s="30"/>
+      <c r="I84" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="J84" s="36"/>
+      <c r="K84" s="37"/>
     </row>
     <row r="85" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="23">
         <v>3</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="C85" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D85" s="32"/>
+        <v>152</v>
+      </c>
+      <c r="C85" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D85" s="34"/>
       <c r="E85" s="25" t="s">
-        <v>158</v>
+        <v>16</v>
       </c>
       <c r="F85" s="25"/>
       <c r="G85" s="25"/>
       <c r="H85" s="25"/>
-      <c r="I85" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="J85" s="29"/>
-      <c r="K85" s="30"/>
+      <c r="I85" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="J85" s="36"/>
+      <c r="K85" s="37"/>
     </row>
     <row r="86" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C86" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D86" s="32"/>
+        <v>153</v>
+      </c>
+      <c r="C86" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D86" s="34"/>
       <c r="E86" s="25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F86" s="25"/>
       <c r="G86" s="25"/>
-      <c r="H86" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="I86" s="28" t="s">
+      <c r="H86" s="25"/>
+      <c r="I86" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="J86" s="29"/>
-      <c r="K86" s="30"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="37"/>
     </row>
     <row r="87" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C87" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="D87" s="27"/>
-      <c r="E87" s="25"/>
+        <v>22</v>
+      </c>
+      <c r="C87" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D87" s="34"/>
+      <c r="E87" s="25" t="s">
+        <v>158</v>
+      </c>
       <c r="F87" s="25"/>
       <c r="G87" s="25"/>
-      <c r="H87" s="25"/>
-      <c r="I87" s="28" t="s">
+      <c r="H87" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="I87" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="J87" s="29"/>
-      <c r="K87" s="30"/>
-    </row>
-    <row r="90" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="22" t="s">
+      <c r="J87" s="36"/>
+      <c r="K87" s="37"/>
+    </row>
+    <row r="88" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="23">
+        <v>5</v>
+      </c>
+      <c r="B88" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C88" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="D88" s="42"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="25"/>
+      <c r="H88" s="25"/>
+      <c r="I88" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="J88" s="36"/>
+      <c r="K88" s="37"/>
+    </row>
+    <row r="91" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B90" s="23" t="s">
+      <c r="B91" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C90" s="22" t="s">
+      <c r="C91" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D90" s="37" t="s">
+      <c r="D91" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="E91" s="43"/>
+      <c r="F91" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G91" s="45"/>
+      <c r="H91" s="46">
+        <v>44377</v>
+      </c>
+      <c r="I91" s="47"/>
+      <c r="J91" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="K91" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="48"/>
+      <c r="C92" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D92" s="43"/>
+      <c r="E92" s="43"/>
+      <c r="F92" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G92" s="45"/>
+      <c r="H92" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="I92" s="50"/>
+      <c r="J92" s="50"/>
+      <c r="K92" s="47"/>
+    </row>
+    <row r="93" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" s="48"/>
+      <c r="E93" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G93" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H93" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I93" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="J93" s="51"/>
+      <c r="K93" s="45"/>
+    </row>
+    <row r="94" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="23">
+        <v>1</v>
+      </c>
+      <c r="B94" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="E90" s="37"/>
-      <c r="F90" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G90" s="39"/>
-      <c r="H90" s="40">
-        <v>44377</v>
-      </c>
-      <c r="I90" s="41"/>
-      <c r="J90" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="K90" s="23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B91" s="42"/>
-      <c r="C91" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="D91" s="37"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G91" s="39"/>
-      <c r="H91" s="43" t="s">
-        <v>182</v>
-      </c>
-      <c r="I91" s="44"/>
-      <c r="J91" s="44"/>
-      <c r="K91" s="41"/>
-    </row>
-    <row r="92" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="22" t="s">
+      <c r="C94" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="D94" s="38"/>
+      <c r="E94" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="F94" s="24"/>
+      <c r="G94" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="H94" s="24"/>
+      <c r="I94" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="J94" s="40"/>
+      <c r="K94" s="41"/>
+    </row>
+    <row r="95" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="5">
         <v>2</v>
       </c>
-      <c r="B92" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C92" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D92" s="42"/>
-      <c r="E92" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F92" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G92" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H92" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I92" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="J92" s="45"/>
-      <c r="K92" s="39"/>
-    </row>
-    <row r="93" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="23">
-        <v>1</v>
-      </c>
-      <c r="B93" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C93" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="D93" s="33"/>
-      <c r="E93" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="F93" s="24"/>
-      <c r="G93" s="24" t="s">
+      <c r="B95" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C95" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="D95" s="42"/>
+      <c r="E95" s="25" t="s">
         <v>174</v>
-      </c>
-      <c r="H93" s="24"/>
-      <c r="I93" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="J93" s="35"/>
-      <c r="K93" s="36"/>
-    </row>
-    <row r="94" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="5">
-        <v>2</v>
-      </c>
-      <c r="B94" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="C94" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D94" s="27"/>
-      <c r="E94" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
-      <c r="H94" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="I94" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="J94" s="29"/>
-      <c r="K94" s="30"/>
-    </row>
-    <row r="95" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="23">
-        <v>3</v>
-      </c>
-      <c r="B95" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C95" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="D95" s="32"/>
-      <c r="E95" s="25" t="s">
-        <v>191</v>
       </c>
       <c r="F95" s="25"/>
       <c r="G95" s="25"/>
       <c r="H95" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="I95" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="J95" s="29"/>
-      <c r="K95" s="30"/>
+        <v>173</v>
+      </c>
+      <c r="I95" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="J95" s="36"/>
+      <c r="K95" s="37"/>
     </row>
     <row r="96" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C96" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D96" s="33"/>
+        <v>184</v>
+      </c>
+      <c r="D96" s="34"/>
       <c r="E96" s="25" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="F96" s="25"/>
       <c r="G96" s="25"/>
       <c r="H96" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="I96" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="J96" s="29"/>
-      <c r="K96" s="30"/>
+        <v>173</v>
+      </c>
+      <c r="I96" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="J96" s="36"/>
+      <c r="K96" s="37"/>
     </row>
     <row r="97" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="C97" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="D97" s="32"/>
+        <v>131</v>
+      </c>
+      <c r="C97" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D97" s="38"/>
       <c r="E97" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F97" s="25"/>
       <c r="G97" s="25"/>
-      <c r="H97" s="25"/>
-      <c r="I97" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="J97" s="29"/>
-      <c r="K97" s="30"/>
+      <c r="H97" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="I97" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="J97" s="36"/>
+      <c r="K97" s="37"/>
     </row>
     <row r="98" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="C98" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="D98" s="32"/>
+        <v>191</v>
+      </c>
+      <c r="C98" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D98" s="34"/>
       <c r="E98" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F98" s="25"/>
       <c r="G98" s="25"/>
       <c r="H98" s="25"/>
-      <c r="I98" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="J98" s="29"/>
-      <c r="K98" s="30"/>
+      <c r="I98" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="J98" s="36"/>
+      <c r="K98" s="37"/>
+    </row>
+    <row r="99" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="23">
+        <v>6</v>
+      </c>
+      <c r="B99" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="C99" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D99" s="34"/>
+      <c r="E99" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="F99" s="25"/>
+      <c r="G99" s="25"/>
+      <c r="H99" s="25"/>
+      <c r="I99" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="J99" s="36"/>
+      <c r="K99" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="192">
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="I98:K98"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="I93:K93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="I94:K94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="I95:K95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="I96:K96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="I97:K97"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="F91:G91"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="I92:K92"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="I87:K87"/>
+  <mergeCells count="194">
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="I76:K76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="I77:K77"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="I70:K70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="I71:K71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="I73:K73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="I74:K74"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="H68:K68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="I69:K69"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="I75:K75"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="I59:K59"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="I60:K60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="I61:K61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="H81:K81"/>
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="I82:K82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="I83:K83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="I84:K84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="I85:K85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="I86:K86"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="I81:K81"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="D1:E1"/>
@@ -3695,132 +3816,51 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="I13:K13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="I88:K88"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="I61:K61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="I62:K62"/>
     <mergeCell ref="C63:D63"/>
     <mergeCell ref="I63:K63"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="I59:K59"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H67:K67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="I68:K68"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="I74:K74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="I75:K75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="I76:K76"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="I69:K69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="I70:K70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="I71:K71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="I72:K72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="I73:K73"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="I83:K83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="I84:K84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="I85:K85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="I86:K86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="I87:K87"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="I64:K64"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="F91:G91"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="F92:G92"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="I93:K93"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="I99:K99"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="I94:K94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="I95:K95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="I96:K96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="I97:K97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="I98:K98"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>